<commit_message>
merging all updated files on v5.6.0-rc.5
</commit_message>
<xml_diff>
--- a/Excel_Files/SampleTest.xlsx
+++ b/Excel_Files/SampleTest.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nmaduru\Documents\CDMNextAutomation\Cucumber_project\Excel_Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NadiyaMaduru\OneDrive - SHRAVAS TECHNOLOGIES INDIA PRIVATE LIMITED\Documents\CDMNextAutomation\Cucumber_project\Excel_Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B974FB19-6BD1-4020-92C4-4920628D89EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCC804E8-2871-476C-9F44-C0FC983B8C27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet0" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet2" r:id="rId6" sheetId="3"/>
+    <sheet name="Sheet0" sheetId="2" state="hidden" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="3" state="hidden" r:id="rId3"/>
     <sheet name="Sheet3" r:id="rId7" sheetId="4"/>
     <sheet name="Sheet4" r:id="rId8" sheetId="5"/>
     <sheet name="Sheet5" r:id="rId9" sheetId="6"/>
@@ -30,57 +30,26 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
-    <t xml:space="preserve">	Region	Subnational	Frequency	Unit	Source	Status	Series ID	SR Code	Mnemonic	Function Description	First Obs. Date	Last Obs. Date	Last Update Time	Series remarks	Suggestions	Mean	Variance	Standard Deviation	Skewness	Kurtosis	Coefficient Variation	Min	Max	Median	No. of Obs	01-03-21	01-04-21	01-05-21	01-06-21	01-07-21	01-08-21	01-09-21	01-10-21	01-11-21	01-12-21
-Industrial Production Index: YoY: Monthly: sa: Japan	Japan		Monthly	%	CEIC Data	Active	249416501 (JBAAAAAAAA)	SR4138501	JP.IPI.VO.SA-YoY-M		01-01-54	01-12-21	30/01/2022	1. CEIC calculates Industrial Production Index Growth from monthly Industrial Production Index.   2. The Ministry of Economy, Trade and Industry provides Industrial Production Index with base 2015=100.   3. Industrial Production Index covers Manufacturing and Mining sectors only.   4. Industrial Production Index Growth prior to January 1979 is calculated from Industrial Production Index with base 2010=100 sourced from the International Monetary Fund.		8.270886020999999	88.9503432716893	9.431348963519975	0.4534142856430915	-1.3528188679937951	1.1403069682708151	-2.56684492	22.96296296	5.318976275000001	10	1.03950104	15.87485516	21.11398964	22.96296296	13.27944573	7.13476784	-2.29257642	-2.56684492	3.50318471	2.65957447</t>
+    <t>=CEIC.LINK("b68f2314-4b51-4e62-8dc1-1b9615c076a8", "Series")	Region	Subnational	Frequency	Unit	Source	Status	Series ID	SR Code	Trade Code	Mnemonic	Function Description	First Obs. Date	Last Obs. Date	Last Update Time	Series remarks	Suggestions	Mean	Variance	Standard Deviation	Skewness	Kurtosis	Coefficient Variation	Min	Max	Median	Sum	Subtract	No. of Obs	01/2022	02/2022	03/2022	04/2022	05/2022	06/2022	07/2022	08/2022	09/2022	10/2022
+Industrial Production Index: YoY: Monthly: sa: Japan	Japan		Monthly	%	CEIC Data	Active	249416501 (JBAAAAAAAA)	SR4138501		JP.IPI.VO.SA-YoY-M		01/1954	10/2022	29/11/2022	1. CEIC calculates Industrial Production Index Growth from monthly Industrial Production Index.   2. The Ministry of Economy, Trade and Industry provides Industrial Production Index with base 2015=100.   3. Industrial Production Index covers Manufacturing and Mining sectors only.   4. Industrial Production Index Growth prior to January 1979 is calculated from Industrial Production Index with base 2010=100 sourced from the International Monetary Fund.		0.42581601499999994	19.199767446149636	4.3817539235047915	1.0685994855023717	0.6642617061127201	10.290251585546383	-4.65872156	9.56618465	-1.022720485	4.258160149999999	-14.22490621	10	-1.565762	0.52246604	-0.82219938	-3.35365854	-4.65872156	-2.83114257	-1.22324159	4.15800416	9.56618465	4.46623094</t>
   </si>
   <si>
-    <t xml:space="preserve">	Region	Subnational	Frequency	Unit	Source	Status	Series ID	SR Code	Mnemonic	Function Description	First Obs. Date	Last Obs. Date	Last Update Time	Series remarks	Suggestions	Mean	Variance	Standard Deviation	Skewness	Kurtosis	Coefficient Variation	Min	Max	Median	No. of Obs	09/2021	10/2021	11/2021	12/2021	01/2022	02/2022	03/2022	04/2022	05/2022	06/2022
-Industrial Production Index: YoY: Monthly: sa: Japan	Japan		Monthly	%	CEIC Data	Active	249416501 (JBAAAAAAAA)	SR4138501	JP.IPI.VO.SA-YoY-M		01/1954	06/2022	15/08/2022	1. CEIC calculates Industrial Production Index Growth from monthly Industrial Production Index.   2. The Ministry of Economy, Trade and Industry provides Industrial Production Index with base 2015=100.   3. Industrial Production Index covers Manufacturing and Mining sectors only.   4. Industrial Production Index Growth prior to January 1979 is calculated from Industrial Production Index with base 2010=100 sourced from the International Monetary Fund.		-1.12816811	5.721561168577328	2.3919785050408224	0.4502085166078148	-0.5379894576169306	-2.120232334027614	-4.65872156	2.76595745	-1.69197191	10	-1.8558952	-1.81818182	2.33545648	2.76595745	-1.565762	0.52246604	-0.82219938	-3.35365854	-4.65872156	-2.83114257</t>
+    <t>=CEIC.LINK("e889093d-df8e-4118-a6e8-886ad6166035", "Series")	Region	Subnational	Frequency	Unit	Source	Status	Series ID	SR Code	Trade Code	Mnemonic	Function Description	First Obs. Date	Last Obs. Date	Last Update Time	Series remarks	Suggestions	Mean	Variance	Standard Deviation	Skewness	Kurtosis	Coefficient Variation	Min	Max	Median	Sum	Subtract	No. of Obs	01/2022	02/2022	03/2022	04/2022	05/2022	06/2022	07/2022	08/2022	09/2022	10/2022
+Industrial Production Index: YoY: Monthly: sa: Japan	Japan		Monthly	%	CEIC Data	Active	249416501 (JBAAAAAAAA)	SR4138501		JP.IPI.VO.SA-YoY-M		01/1954	10/2022	29/11/2022	1. CEIC calculates Industrial Production Index Growth from monthly Industrial Production Index.   2. The Ministry of Economy, Trade and Industry provides Industrial Production Index with base 2015=100.   3. Industrial Production Index covers Manufacturing and Mining sectors only.   4. Industrial Production Index Growth prior to January 1979 is calculated from Industrial Production Index with base 2010=100 sourced from the International Monetary Fund.		0.42581601499999994	19.199767446149636	4.3817539235047915	1.0685994855023717	0.6642617061127201	10.290251585546383	-4.65872156	9.56618465	-1.022720485	4.258160149999999	-14.22490621	10	-1.565762	0.52246604	-0.82219938	-3.35365854	-4.65872156	-2.83114257	-1.22324159	4.15800416	9.56618465	4.46623094</t>
   </si>
   <si>
-    <t xml:space="preserve">	Region	Subnational	Frequency	Unit	Source	Status	Series ID	SR Code	Mnemonic	Function Description	First Obs. Date	Last Obs. Date	Last Update Time	Series remarks	Suggestions	Mean	Variance	Standard Deviation	Skewness	Kurtosis	Coefficient Variation	Min	Max	Median	No. of Obs	11/2021	12/2021	01/2022	02/2022	03/2022	04/2022	05/2022	06/2022	07/2022	08/2022
-Industrial Production Index: YoY: Monthly: sa: Japan	Japan		Monthly	%	CEIC Data	Active	249416501 (JBAAAAAAAA)	SR4138501	JP.IPI.VO.SA-YoY-M		01/1954	08/2022	29/09/2022	1. CEIC calculates Industrial Production Index Growth from monthly Industrial Production Index.   2. The Ministry of Economy, Trade and Industry provides Industrial Production Index with base 2015=100.   3. Industrial Production Index covers Manufacturing and Mining sectors only.   4. Industrial Production Index Growth prior to January 1979 is calculated from Industrial Production Index with base 2010=100 sourced from the International Monetary Fund.		-0.5400492240000002	7.535407137359178	2.745069605193861	0.12161038180917919	-1.1992943366162025	-5.082998888252934	-4.65872156	3.43035343	-1.022720485	10	2.33545648	2.76595745	-1.565762	0.52246604	-0.82219938	-3.35365854	-4.65872156	-2.83114257	-1.22324159	3.43035343</t>
+    <t>=CEIC.LINK("0d4bc7c3-ae44-4367-8d19-9a74232f3c24", "Series")	Region	Subnational	Frequency	Unit	Source	Status	Series ID	SR Code	Trade Code	Mnemonic	Function Description	First Obs. Date	Last Obs. Date	Last Update Time	Series remarks	Suggestions	Mean	Variance	Standard Deviation	Skewness	Kurtosis	Coefficient Variation	Min	Max	Median	Sum	Subtract	No. of Obs	01/2022	02/2022	03/2022	04/2022	05/2022	06/2022	07/2022	08/2022	09/2022	10/2022
+Industrial Production Index: YoY: Monthly: sa: Japan	Japan		Monthly	%	CEIC Data	Active	249416501 (JBAAAAAAAA)	SR4138501		JP.IPI.VO.SA-YoY-M		01/1954	10/2022	29/11/2022	1. CEIC calculates Industrial Production Index Growth from monthly Industrial Production Index.   2. The Ministry of Economy, Trade and Industry provides Industrial Production Index with base 2015=100.   3. Industrial Production Index covers Manufacturing and Mining sectors only.   4. Industrial Production Index Growth prior to January 1979 is calculated from Industrial Production Index with base 2010=100 sourced from the International Monetary Fund.		0.42581601499999994	19.199767446149636	4.3817539235047915	1.0685994855023717	0.6642617061127201	10.290251585546383	-4.65872156	9.56618465	-1.022720485	4.258160149999999	-14.22490621	10	-1.565762	0.52246604	-0.82219938	-3.35365854	-4.65872156	-2.83114257	-1.22324159	4.15800416	9.56618465	4.46623094</t>
   </si>
   <si>
-    <t xml:space="preserve">	Industrial Production Index: YoY: Monthly: sa: Japan
-Region	Japan
-Subnational	
-Frequency	Monthly
-Unit	%
-Source	CEIC Data
-Status	Active
-Series ID	249416501 (JBAAAAAAAA)
-SR Code	SR4138501
-Trade Code	
-Mnemonic	JP.IPI.VO.SA-YoY-M
-Function Description	
-First Obs. Date	01/1954
-Last Obs. Date	08/2022
-Last Update Time	17/10/2022
-Series remarks	1. CEIC calculates Industrial Production Index Growth from monthly Industrial Production Index.   2. The Ministry of Economy, Trade and Industry provides Industrial Production Index with base 2015=100.   3. Industrial Production Index covers Manufacturing and Mining sectors only.   4. Industrial Production Index Growth prior to January 1979 is calculated from Industrial Production Index with base 2010=100 sourced from the International Monetary Fund.
-Suggestions	
-Mean	-0.46728415100000015
-Variance	8.230369449085474
-Standard Deviation	2.868862047761355
-Skewness	0.2531832579397403
-Kurtosis	-0.9861905193339364
-Coefficient Variation	-6.1394379450317675
-Min	-4.65872156
-Max	4.15800416
-Median	-1.022720485
-No. of Obs	10
-11/2021	2.33545648
-12/2021	2.76595745
-01/2022	-1.565762
-02/2022	0.52246604
-03/2022	-0.82219938
-04/2022	-3.35365854
-05/2022	-4.65872156
-06/2022	-2.83114257
-07/2022	-1.22324159
-08/2022	4.15800416</t>
+    <t>=CEIC.LINK("66003d0b-f06b-4830-871e-159741ac37d4", "Series")	Region	Subnational	Frequency	Unit	Source	Status	Series ID	SR Code	Trade Code	Mnemonic	Function Description	First Obs. Date	Last Obs. Date	Last Update Time	Series remarks	Suggestions	Mean	Variance	Standard Deviation	Skewness	Kurtosis	Coefficient Variation	Min	Max	Median	Sum	Subtract	No. of Obs	01/2022	02/2022	03/2022	04/2022	05/2022	06/2022	07/2022	08/2022	09/2022	10/2022
+Industrial Production Index: YoY: Monthly: sa: Japan	Japan		Monthly	%	CEIC Data	Active	249416501 (JBAAAAAAAA)	SR4138501		JP.IPI.VO.SA-YoY-M		01/1954	10/2022	29/11/2022	1. CEIC calculates Industrial Production Index Growth from monthly Industrial Production Index.   2. The Ministry of Economy, Trade and Industry provides Industrial Production Index with base 2015=100.   3. Industrial Production Index covers Manufacturing and Mining sectors only.   4. Industrial Production Index Growth prior to January 1979 is calculated from Industrial Production Index with base 2010=100 sourced from the International Monetary Fund.		0.42581601499999994	19.199767446149636	4.3817539235047915	1.0685994855023717	0.6642617061127201	10.290251585546383	-4.65872156	9.56618465	-1.022720485	4.258160149999999	-14.22490621	10	-1.565762	0.52246604	-0.82219938	-3.35365854	-4.65872156	-2.83114257	-1.22324159	4.15800416	9.56618465	4.46623094</t>
+  </si>
+  <si>
+    <t>=CEIC.LINK("1da2e350-408c-49f6-9230-12f3f516aa11", "Series")	Region	Subnational	Frequency	Unit	Source	Status	Series ID	SR Code	Trade Code	Mnemonic	Function Description	First Obs. Date	Last Obs. Date	Last Update Time	Series remarks	Suggestions	Mean	Variance	Standard Deviation	Skewness	Kurtosis	Coefficient Variation	Min	Max	Median	Sum	Subtract	No. of Obs	01/2022	02/2022	03/2022	04/2022	05/2022	06/2022	07/2022	08/2022	09/2022	10/2022
+Industrial Production Index: YoY: Monthly: sa: Japan	Japan		Monthly	%	CEIC Data	Active	249416501 (JBAAAAAAAA)	SR4138501		JP.IPI.VO.SA-YoY-M		01/1954	10/2022	29/11/2022	1. CEIC calculates Industrial Production Index Growth from monthly Industrial Production Index.   2. The Ministry of Economy, Trade and Industry provides Industrial Production Index with base 2015=100.   3. Industrial Production Index covers Manufacturing and Mining sectors only.   4. Industrial Production Index Growth prior to January 1979 is calculated from Industrial Production Index with base 2010=100 sourced from the International Monetary Fund.		0.42581601499999994	19.199767446149636	4.3817539235047915	1.0685994855023717	0.6642617061127201	10.290251585546383	-4.65872156	9.56618465	-1.022720485	4.258160149999999	-14.22490621	10	-1.565762	0.52246604	-0.82219938	-3.35365854	-4.65872156	-2.83114257	-1.22324159	4.15800416	9.56618465	4.46623094</t>
   </si>
 </sst>
 </file>
@@ -399,12 +368,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <dimension ref="B1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1"/>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -413,11 +391,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -428,21 +406,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1"/>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -453,14 +424,7 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1"/>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
@@ -472,14 +436,7 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1"/>
-      <c r="B1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
@@ -491,14 +448,7 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1"/>
-      <c r="B1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>